<commit_message>
merged login, program and dashboard module
</commit_message>
<xml_diff>
--- a/tests/TestData/PlayWright_Group2_Data.xlsx
+++ b/tests/TestData/PlayWright_Group2_Data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rathna\PlayWright_Group2_LMS_BDD_Project\tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4871705A-B66F-44AB-9FED-9E5FEF86E29B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924F400E-E301-4970-B5C7-8ADF6F4E36A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E6FF7971-DA04-49AA-8DA4-D74C41129B5A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{E6FF7971-DA04-49AA-8DA4-D74C41129B5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="InvalidLogin" sheetId="2" r:id="rId2"/>
+    <sheet name="Dashboard" sheetId="2" r:id="rId2"/>
+    <sheet name="Program" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
   <si>
     <t>playwrightuser@gmail.com</t>
   </si>
@@ -89,6 +90,57 @@
   </si>
   <si>
     <t xml:space="preserve">Please enter your user name </t>
+  </si>
+  <si>
+    <t>expectedValue</t>
+  </si>
+  <si>
+    <t>nth</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LMS - Learning Management System </t>
+  </si>
+  <si>
+    <t>navBarText</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LMS - Learning Management System ProgramBatchClassLogout</t>
+  </si>
+  <si>
+    <t>program</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>batch</t>
+  </si>
+  <si>
+    <t>Batch</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>logout</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>expected</t>
+  </si>
+  <si>
+    <t>programModule</t>
+  </si>
+  <si>
+    <t>Manage Program</t>
   </si>
 </sst>
 </file>
@@ -456,7 +508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC6DC461-3933-4E84-8F9A-EDEFE7A41CAB}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -567,10 +619,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71104904-0BD0-410B-BA08-4F962794E43E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -578,7 +630,204 @@
     <col min="1" max="1" width="27.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.81640625" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE17ACF-C6C7-40F7-BE92-0D5B7CEEB2BA}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Andd new User Completed
</commit_message>
<xml_diff>
--- a/tests/TestData/PlayWright_Group2_Data.xlsx
+++ b/tests/TestData/PlayWright_Group2_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amreennaziasyed/Playwright_Group2_LMS_BDD_Project/tests/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9FEEE8-9C7F-6E49-AD46-35CA4AD31C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7066B68-C824-8B4F-BBA4-96A167D1F299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{E6FF7971-DA04-49AA-8DA4-D74C41129B5A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{E6FF7971-DA04-49AA-8DA4-D74C41129B5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>playwrightuser@gmail.com</t>
   </si>
@@ -149,10 +149,13 @@
     <t>validInput</t>
   </si>
   <si>
-    <t>playwrightwithJava</t>
-  </si>
-  <si>
     <t>validatetextbox</t>
+  </si>
+  <si>
+    <t>python</t>
+  </si>
+  <si>
+    <t>programming language</t>
   </si>
 </sst>
 </file>
@@ -776,7 +779,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -800,7 +803,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>32</v>
@@ -814,10 +817,10 @@
         <v>36</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Revert "Merge pull request #23 from AmreenNazia/Amreen"
This reverts commit dc84bbe14c7bee1ec2aef254667d9c30cc7772aa, reversing
changes made to 41563d172f37bb28e57989b8b005124f28effd31.
</commit_message>
<xml_diff>
--- a/tests/TestData/PlayWright_Group2_Data.xlsx
+++ b/tests/TestData/PlayWright_Group2_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amreennaziasyed/Playwright_Group2_LMS_BDD_Project/tests/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E559B93-F70D-3047-821D-FF4EE012EECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7705C4-1B6E-F840-A8CD-48948324390D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{E6FF7971-DA04-49AA-8DA4-D74C41129B5A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
   <si>
     <t>playwrightuser@gmail.com</t>
   </si>
@@ -153,6 +153,9 @@
     <t>validatetextbox</t>
   </si>
   <si>
+    <t>DA-course</t>
+  </si>
+  <si>
     <t>classTopic</t>
   </si>
   <si>
@@ -169,34 +172,13 @@
   </si>
   <si>
     <t>Scrum master</t>
-  </si>
-  <si>
-    <t>editprogram</t>
-  </si>
-  <si>
-    <t>SearchUpdatedName</t>
-  </si>
-  <si>
-    <t>searchCreatedName</t>
-  </si>
-  <si>
-    <t>Devops</t>
-  </si>
-  <si>
-    <t>Cybersecurity</t>
-  </si>
-  <si>
-    <t>testing</t>
-  </si>
-  <si>
-    <t>BDD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,18 +207,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FFC586C0"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -259,7 +229,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -267,8 +237,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -831,21 +799,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE17ACF-C6C7-40F7-BE92-0D5B7CEEB2BA}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
     <col min="2" max="2" width="25.5" customWidth="1"/>
-    <col min="3" max="4" width="42" style="3" customWidth="1"/>
-    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -855,14 +823,8 @@
       <c r="C1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>37</v>
       </c>
@@ -872,76 +834,58 @@
       <c r="C2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>47</v>
-      </c>
+      <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -966,13 +910,13 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="24" x14ac:dyDescent="0.3">
@@ -980,13 +924,13 @@
         <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated pagination and sorting of class
</commit_message>
<xml_diff>
--- a/tests/TestData/PlayWright_Group2_Data.xlsx
+++ b/tests/TestData/PlayWright_Group2_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amreennaziasyed/Playwright_Group2_LMS_BDD_Project/tests/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rathna\PlayWright_Group2_LMS_BDD_Project\tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E559B93-F70D-3047-821D-FF4EE012EECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1145D4B-4134-4F73-A671-B273A731A7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{E6FF7971-DA04-49AA-8DA4-D74C41129B5A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{E6FF7971-DA04-49AA-8DA4-D74C41129B5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
   <si>
     <t>playwrightuser@gmail.com</t>
   </si>
@@ -190,13 +190,19 @@
   </si>
   <si>
     <t>BDD</t>
+  </si>
+  <si>
+    <t>DeleteProgram</t>
+  </si>
+  <si>
+    <t>DelTestOne</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -590,15 +596,15 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.1640625" customWidth="1"/>
+    <col min="1" max="1" width="27.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -612,7 +618,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -623,7 +629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="24.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="24.5" customHeight="1">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -637,7 +643,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -651,7 +657,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -662,7 +668,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="29">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -676,7 +682,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -703,15 +709,15 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -728,7 +734,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -742,7 +748,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -756,7 +762,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -773,7 +779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -790,7 +796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -807,7 +813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -834,18 +840,18 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="23.5"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="25.5" customWidth="1"/>
+    <col min="2" max="2" width="25.453125" customWidth="1"/>
     <col min="3" max="4" width="42" style="3" customWidth="1"/>
     <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -862,7 +868,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
         <v>37</v>
       </c>
@@ -874,7 +880,7 @@
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
         <v>36</v>
       </c>
@@ -886,7 +892,7 @@
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" s="5" t="s">
         <v>44</v>
       </c>
@@ -903,39 +909,43 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
+      <c r="A5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
     </row>
@@ -953,15 +963,15 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="23.5">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -975,7 +985,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="23.5">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Deleted clear Screenshot.js file from utils
</commit_message>
<xml_diff>
--- a/tests/TestData/PlayWright_Group2_Data.xlsx
+++ b/tests/TestData/PlayWright_Group2_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amreennaziasyed/Playwright_Group2_LMS_BDD_Project/tests/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0403A210-9D03-EF48-8998-9A8562DC1F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7884DF-9AEF-144B-A462-6BA1DBADEE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{E6FF7971-DA04-49AA-8DA4-D74C41129B5A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>playwrightuser@gmail.com</t>
   </si>
@@ -180,22 +180,19 @@
     <t>searchCreatedName</t>
   </si>
   <si>
-    <t>Devops</t>
-  </si>
-  <si>
     <t>Cybersecurity</t>
   </si>
   <si>
     <t>testing</t>
   </si>
   <si>
-    <t>BDD</t>
-  </si>
-  <si>
     <t>DeleteProgram</t>
   </si>
   <si>
-    <t>DelTestOne</t>
+    <t>OOPs concepts</t>
+  </si>
+  <si>
+    <t>corejava</t>
   </si>
 </sst>
 </file>
@@ -840,7 +837,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -885,7 +882,7 @@
         <v>36</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>50</v>
@@ -897,24 +894,24 @@
         <v>44</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="D4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated class Edit with DataDriven
</commit_message>
<xml_diff>
--- a/tests/TestData/PlayWright_Group2_Data.xlsx
+++ b/tests/TestData/PlayWright_Group2_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rathna\PlayWright_Group2_LMS_BDD_Project\tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1145D4B-4134-4F73-A671-B273A731A7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FEFE26-7CD7-460B-B215-C8D9ECEF9336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{E6FF7971-DA04-49AA-8DA4-D74C41129B5A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{E6FF7971-DA04-49AA-8DA4-D74C41129B5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
   <si>
     <t>playwrightuser@gmail.com</t>
   </si>
@@ -196,13 +196,46 @@
   </si>
   <si>
     <t>DelTestOne</t>
+  </si>
+  <si>
+    <t>ValidEditData</t>
+  </si>
+  <si>
+    <t>Saranya M</t>
+  </si>
+  <si>
+    <t>ClassDesc</t>
+  </si>
+  <si>
+    <t>OptionalValid</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Playwright with Appium</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>c:/user/Notes</t>
+  </si>
+  <si>
+    <t>c:/Recordings</t>
+  </si>
+  <si>
+    <t>Recording</t>
+  </si>
+  <si>
+    <t>NumericOrAlphaData</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,12 +257,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF1F1F1F"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="18"/>
@@ -265,7 +292,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -274,7 +301,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -839,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE17ACF-C6C7-40F7-BE92-0D5B7CEEB2BA}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="23.5"/>
@@ -884,7 +910,7 @@
       <c r="A3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>47</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -893,19 +919,19 @@
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>48</v>
       </c>
     </row>
@@ -957,10 +983,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9E0E79-7EE5-814B-B938-A957080C7691}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
@@ -971,36 +997,90 @@
     <col min="4" max="4" width="18.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.5">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="23.5">
-      <c r="A2" s="3" t="s">
+      <c r="E1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5">
+        <v>23423</v>
+      </c>
+      <c r="F5">
+        <v>435254</v>
+      </c>
+      <c r="G5">
+        <v>23452</v>
+      </c>
+      <c r="H5">
+        <v>123515</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tested 114 test cases
</commit_message>
<xml_diff>
--- a/tests/TestData/PlayWright_Group2_Data.xlsx
+++ b/tests/TestData/PlayWright_Group2_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rathna\PlayWright_Group2_LMS_BDD_Project\tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8372E5D9-264C-4D2B-9481-83D58DE55A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4460EC33-F492-45F5-9056-861492971A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{E6FF7971-DA04-49AA-8DA4-D74C41129B5A}"/>
   </bookViews>
@@ -195,9 +195,6 @@
     <t>DeleteProgram</t>
   </si>
   <si>
-    <t>DelTestOne</t>
-  </si>
-  <si>
     <t>ValidEditData</t>
   </si>
   <si>
@@ -229,6 +226,9 @@
   </si>
   <si>
     <t>NumericOrAlphaData</t>
+  </si>
+  <si>
+    <t>DelTestSix</t>
   </si>
 </sst>
 </file>
@@ -866,7 +866,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="23.5"/>
@@ -940,7 +940,7 @@
         <v>51</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1011,16 +1011,16 @@
         <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1039,32 +1039,32 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
         <v>53</v>
-      </c>
-      <c r="D3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
         <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" t="s">
         <v>60</v>
-      </c>
-      <c r="H4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5">
         <v>23423</v>

</xml_diff>